<commit_message>
created door class and methods - all tests pass
</commit_message>
<xml_diff>
--- a/door_notes.xlsx
+++ b/door_notes.xlsx
@@ -47,9 +47,6 @@
     <t>Method Type</t>
   </si>
   <si>
-    <t>read</t>
-  </si>
-  <si>
     <t>reads the inscription on the door</t>
   </si>
   <si>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>unlocked door</t>
+  </si>
+  <si>
+    <t>inscription</t>
   </si>
 </sst>
 </file>
@@ -466,7 +466,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5:G6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,171 +503,171 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" t="s">
         <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" t="s">
         <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>28</v>
-      </c>
-      <c r="G8" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>